<commit_message>
fixed tab name to standardize
</commit_message>
<xml_diff>
--- a/MI_Montmorency/MI_Montmorency_GE20_cleaned.xlsx
+++ b/MI_Montmorency/MI_Montmorency_GE20_cleaned.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITREPOS\gh_kessler\openelections_work\MI_Montmorency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFFDE62-3921-4FC8-8920-C020F52CCEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB2AF61-DABE-46F0-9FE7-D4C23FDC4BDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="1540" windowWidth="29760" windowHeight="16750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20090" yWindow="1540" windowWidth="14810" windowHeight="16750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="total_reg_and_ballots" sheetId="2" r:id="rId1"/>
+    <sheet name="total_reg_and_cast" sheetId="2" r:id="rId1"/>
     <sheet name="straightparty" sheetId="3" r:id="rId2"/>
     <sheet name="presidential" sheetId="4" r:id="rId3"/>
     <sheet name="ussenate" sheetId="5" r:id="rId4"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>

</xml_diff>